<commit_message>
Its really bad but it works now!
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -43,12 +43,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -61,16 +67,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -87,13 +93,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -113,6 +119,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -312,17 +319,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="19050" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -349,10 +356,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Aptos Narrow"/>
-            <a:ea typeface="Aptos Narrow"/>
-            <a:cs typeface="Aptos Narrow"/>
-            <a:sym typeface="Aptos Narrow"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -591,12 +598,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="19050" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -873,7 +880,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -900,10 +907,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Aptos Narrow"/>
-            <a:ea typeface="Aptos Narrow"/>
-            <a:cs typeface="Aptos Narrow"/>
-            <a:sym typeface="Aptos Narrow"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1169,11 +1176,11 @@
     <row r="2" ht="16" customHeight="1">
       <c r="A2" s="4">
         <f t="shared" si="0" ref="A2:A60">RAND()*(PI()/2--PI()/2)+-PI()/2</f>
-        <v>0.707015753759852</v>
+        <v>-1.55264517009283</v>
       </c>
       <c r="B2" s="4">
         <f>SIN(A2)</f>
-        <v>0.649567733279384</v>
+        <v>-0.999835272277924</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1182,11 +1189,11 @@
     <row r="3" ht="16" customHeight="1">
       <c r="A3" s="4">
         <f t="shared" si="0"/>
-        <v>-1.5322880946095</v>
+        <v>-1.51164741177523</v>
       </c>
       <c r="B3" s="4">
         <f>SIN(A3)</f>
-        <v>-0.999258649645149</v>
+        <v>-0.998251212873234</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1195,11 +1202,11 @@
     <row r="4" ht="16" customHeight="1">
       <c r="A4" s="4">
         <f t="shared" si="0"/>
-        <v>-0.0950020899612317</v>
+        <v>-1.44071427440444</v>
       </c>
       <c r="B4" s="4">
         <f>SIN(A4)</f>
-        <v>-0.0948592491717225</v>
+        <v>-0.991551253585621</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1208,11 +1215,11 @@
     <row r="5" ht="16" customHeight="1">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
-        <v>0.204065145401975</v>
+        <v>-1.36107644455794</v>
       </c>
       <c r="B5" s="4">
         <f>SIN(A5)</f>
-        <v>0.202651791420901</v>
+        <v>-0.978089269673146</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1221,11 +1228,11 @@
     <row r="6" ht="16" customHeight="1">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
-        <v>-1.12860645423664</v>
+        <v>-1.33760113086947</v>
       </c>
       <c r="B6" s="4">
         <f>SIN(A6)</f>
-        <v>-0.903816741433094</v>
+        <v>-0.972932993179809</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1234,11 +1241,11 @@
     <row r="7" ht="16" customHeight="1">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
-        <v>-0.09206700106115651</v>
+        <v>-1.3333642737688</v>
       </c>
       <c r="B7" s="4">
         <f>SIN(A7)</f>
-        <v>-0.09193699108540609</v>
+        <v>-0.971945179251045</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1247,11 +1254,11 @@
     <row r="8" ht="16" customHeight="1">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
-        <v>0.657356426124502</v>
+        <v>-1.22155818595897</v>
       </c>
       <c r="B8" s="4">
         <f>SIN(A8)</f>
-        <v>0.611026309203811</v>
+        <v>-0.939633680039307</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1260,11 +1267,11 @@
     <row r="9" ht="16" customHeight="1">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
-        <v>-0.655075860742698</v>
+        <v>-1.16010647684172</v>
       </c>
       <c r="B9" s="4">
         <f>SIN(A9)</f>
-        <v>-0.609219402781367</v>
+        <v>-0.916845623986508</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1273,11 +1280,11 @@
     <row r="10" ht="16" customHeight="1">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
-        <v>0.972558885148249</v>
+        <v>-1.10212700339652</v>
       </c>
       <c r="B10" s="4">
         <f>SIN(A10)</f>
-        <v>0.826329547704117</v>
+        <v>-0.892170143850664</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1286,11 +1293,11 @@
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
-        <v>-0.0922632823781581</v>
+        <v>-0.892607884429381</v>
       </c>
       <c r="B11" s="4">
         <f>SIN(A11)</f>
-        <v>-0.09213243934471931</v>
+        <v>-0.7787105370352519</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1299,11 +1306,11 @@
     <row r="12" ht="16" customHeight="1">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
-        <v>0.965837591372092</v>
+        <v>-0.887779977643101</v>
       </c>
       <c r="B12" s="4">
         <f>SIN(A12)</f>
-        <v>0.822525566658711</v>
+        <v>-0.77567252500592</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1312,11 +1319,11 @@
     <row r="13" ht="16" customHeight="1">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
-        <v>-1.31552218775672</v>
+        <v>-0.821480952999655</v>
       </c>
       <c r="B13" s="4">
         <f>SIN(A13)</f>
-        <v>-0.967594109014716</v>
+        <v>-0.732155365118606</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1325,11 +1332,11 @@
     <row r="14" ht="16" customHeight="1">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
-        <v>0.240954859528141</v>
+        <v>-0.818135677169967</v>
       </c>
       <c r="B14" s="4">
         <f>SIN(A14)</f>
-        <v>0.238630009243051</v>
+        <v>-0.729872679270525</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1338,11 +1345,11 @@
     <row r="15" ht="16" customHeight="1">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
-        <v>-0.300181540636599</v>
+        <v>-0.817766422424829</v>
       </c>
       <c r="B15" s="4">
         <f>SIN(A15)</f>
-        <v>-0.295693634185059</v>
+        <v>-0.729620213209448</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1351,11 +1358,11 @@
     <row r="16" ht="16" customHeight="1">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
-        <v>0.798016885889347</v>
+        <v>-0.711763679406582</v>
       </c>
       <c r="B16" s="4">
         <f>SIN(A16)</f>
-        <v>0.715973032311242</v>
+        <v>-0.653170263766147</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1364,11 +1371,11 @@
     <row r="17" ht="16" customHeight="1">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
-        <v>-0.878575541261896</v>
+        <v>-0.677063462275784</v>
       </c>
       <c r="B17" s="4">
         <f>SIN(A17)</f>
-        <v>-0.769830501744725</v>
+        <v>-0.626506944559245</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1377,11 +1384,11 @@
     <row r="18" ht="16" customHeight="1">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
-        <v>-0.5560542750230451</v>
+        <v>-0.582616622566775</v>
       </c>
       <c r="B18" s="4">
         <f>SIN(A18)</f>
-        <v>-0.5278390359959521</v>
+        <v>-0.550210765259916</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1390,11 +1397,11 @@
     <row r="19" ht="16" customHeight="1">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
-        <v>-1.00194039001896</v>
+        <v>-0.560235831679888</v>
       </c>
       <c r="B19" s="4">
         <f>SIN(A19)</f>
-        <v>-0.8425177972351811</v>
+        <v>-0.531385992743775</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1403,11 +1410,11 @@
     <row r="20" ht="16" customHeight="1">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
-        <v>0.757305200790064</v>
+        <v>-0.557313167641024</v>
       </c>
       <c r="B20" s="4">
         <f>SIN(A20)</f>
-        <v>0.686965658513039</v>
+        <v>-0.528907850877736</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1416,11 +1423,11 @@
     <row r="21" ht="16" customHeight="1">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
-        <v>-1.52305284547037</v>
+        <v>-0.491372404698041</v>
       </c>
       <c r="B21" s="4">
         <f>SIN(A21)</f>
-        <v>-0.9988604964726731</v>
+        <v>-0.471836362340821</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1429,11 +1436,11 @@
     <row r="22" ht="16" customHeight="1">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
-        <v>0.822910559701061</v>
+        <v>-0.458477269570055</v>
       </c>
       <c r="B22" s="4">
         <f>SIN(A22)</f>
-        <v>0.733128375579751</v>
+        <v>-0.442583146395096</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1442,11 +1449,11 @@
     <row r="23" ht="16" customHeight="1">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
-        <v>-1.0167035775984</v>
+        <v>-0.371010686596956</v>
       </c>
       <c r="B23" s="4">
         <f>SIN(A23)</f>
-        <v>-0.8503781601585469</v>
+        <v>-0.362557537863931</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1455,11 +1462,11 @@
     <row r="24" ht="16" customHeight="1">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
-        <v>1.41043360390347</v>
+        <v>-0.334103649181945</v>
       </c>
       <c r="B24" s="4">
         <f>SIN(A24)</f>
-        <v>0.987169430072627</v>
+        <v>-0.327922514959711</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1468,11 +1475,11 @@
     <row r="25" ht="16" customHeight="1">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
-        <v>0.852549040205963</v>
+        <v>-0.201396792430135</v>
       </c>
       <c r="B25" s="4">
         <f>SIN(A25)</f>
-        <v>0.7529602861318641</v>
+        <v>-0.200038086122084</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1481,11 +1488,11 @@
     <row r="26" ht="16" customHeight="1">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
-        <v>-0.182636485061857</v>
+        <v>-0.166247537710207</v>
       </c>
       <c r="B26" s="4">
         <f>SIN(A26)</f>
-        <v>-0.18162283739831</v>
+        <v>-0.165482796950541</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1494,11 +1501,11 @@
     <row r="27" ht="16" customHeight="1">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
-        <v>-0.450797605522751</v>
+        <v>-0.120456161073362</v>
       </c>
       <c r="B27" s="4">
         <f>SIN(A27)</f>
-        <v>-0.435683597259863</v>
+        <v>-0.120165075471155</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1507,11 +1514,11 @@
     <row r="28" ht="16" customHeight="1">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
-        <v>1.47371270371657</v>
+        <v>-0.0452390141108857</v>
       </c>
       <c r="B28" s="4">
         <f>SIN(A28)</f>
-        <v>0.995291085358873</v>
+        <v>-0.0452235849003798</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1520,11 +1527,11 @@
     <row r="29" ht="16" customHeight="1">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
-        <v>1.06322681348601</v>
+        <v>0.0352097308818991</v>
       </c>
       <c r="B29" s="4">
         <f>SIN(A29)</f>
-        <v>0.873928437013519</v>
+        <v>0.0352024562680305</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1533,11 +1540,11 @@
     <row r="30" ht="16" customHeight="1">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
-        <v>-0.964011236446471</v>
+        <v>0.0407832520479992</v>
       </c>
       <c r="B30" s="4">
         <f>SIN(A30)</f>
-        <v>-0.821485496008037</v>
+        <v>0.0407719473701129</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1546,11 +1553,11 @@
     <row r="31" ht="16" customHeight="1">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
-        <v>-0.751420787899627</v>
+        <v>0.100249807195421</v>
       </c>
       <c r="B31" s="4">
         <f>SIN(A31)</f>
-        <v>-0.682677646373845</v>
+        <v>0.100081972729219</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1559,11 +1566,11 @@
     <row r="32" ht="16" customHeight="1">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
-        <v>-0.8762016000220429</v>
+        <v>0.10378714944317</v>
       </c>
       <c r="B32" s="4">
         <f>SIN(A32)</f>
-        <v>-0.768313169783638</v>
+        <v>0.103600921180101</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1572,11 +1579,11 @@
     <row r="33" ht="16" customHeight="1">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
-        <v>-1.28357056996267</v>
+        <v>0.167655344519459</v>
       </c>
       <c r="B33" s="4">
         <f>SIN(A33)</f>
-        <v>-0.959033487978139</v>
+        <v>0.166871029426912</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1585,11 +1592,11 @@
     <row r="34" ht="16" customHeight="1">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
-        <v>-0.0254963416661772</v>
+        <v>0.257422484885998</v>
       </c>
       <c r="B34" s="4">
         <f>SIN(A34)</f>
-        <v>-0.0254935793827069</v>
+        <v>0.254588815907891</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1598,11 +1605,11 @@
     <row r="35" ht="16" customHeight="1">
       <c r="A35" s="4">
         <f t="shared" si="0"/>
-        <v>0.395702454322271</v>
+        <v>0.276681284955036</v>
       </c>
       <c r="B35" s="4">
         <f>SIN(A35)</f>
-        <v>0.38545645674073</v>
+        <v>0.273164663405542</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1611,11 +1618,11 @@
     <row r="36" ht="16" customHeight="1">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
-        <v>1.27971770175855</v>
+        <v>0.312917599498334</v>
       </c>
       <c r="B36" s="4">
         <f>SIN(A36)</f>
-        <v>0.957934882917582</v>
+        <v>0.307835862059567</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1624,11 +1631,11 @@
     <row r="37" ht="16" customHeight="1">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
-        <v>1.10337202553779</v>
+        <v>0.33315891480419</v>
       </c>
       <c r="B37" s="4">
         <f>SIN(A37)</f>
-        <v>0.892731828111213</v>
+        <v>0.327029873819378</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1637,11 +1644,11 @@
     <row r="38" ht="16" customHeight="1">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
-        <v>0.508403796322951</v>
+        <v>0.358723319742504</v>
       </c>
       <c r="B38" s="4">
         <f>SIN(A38)</f>
-        <v>0.486783547577225</v>
+        <v>0.351079105513783</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1650,11 +1657,11 @@
     <row r="39" ht="16" customHeight="1">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
-        <v>0.05124830271102</v>
+        <v>0.42665640670956</v>
       </c>
       <c r="B39" s="4">
         <f>SIN(A39)</f>
-        <v>0.0512258726643133</v>
+        <v>0.41382926608463</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1663,11 +1670,11 @@
     <row r="40" ht="16" customHeight="1">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
-        <v>0.884524546442273</v>
+        <v>0.439483301741781</v>
       </c>
       <c r="B40" s="4">
         <f>SIN(A40)</f>
-        <v>0.7736137999207769</v>
+        <v>0.425471924620256</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1676,11 +1683,11 @@
     <row r="41" ht="16" customHeight="1">
       <c r="A41" s="4">
         <f t="shared" si="0"/>
-        <v>0.600714555309757</v>
+        <v>0.5710267822587211</v>
       </c>
       <c r="B41" s="4">
         <f>SIN(A41)</f>
-        <v>0.56523207714062</v>
+        <v>0.5404962131048699</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1689,11 +1696,11 @@
     <row r="42" ht="16" customHeight="1">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
-        <v>0.764141247839919</v>
+        <v>0.580127956901073</v>
       </c>
       <c r="B42" s="4">
         <f>SIN(A42)</f>
-        <v>0.691917254624334</v>
+        <v>0.548130963473739</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1702,11 +1709,11 @@
     <row r="43" ht="16" customHeight="1">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
-        <v>-0.6494416548591631</v>
+        <v>0.605417995203174</v>
       </c>
       <c r="B43" s="4">
         <f>SIN(A43)</f>
-        <v>-0.6047418219053</v>
+        <v>0.569105828493248</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1715,11 +1722,11 @@
     <row r="44" ht="16" customHeight="1">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
-        <v>0.570286731776623</v>
+        <v>0.615961761622818</v>
       </c>
       <c r="B44" s="4">
         <f>SIN(A44)</f>
-        <v>0.539873426310056</v>
+        <v>0.577743796680971</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1728,11 +1735,11 @@
     <row r="45" ht="16" customHeight="1">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
-        <v>0.289549687973682</v>
+        <v>0.78143219912312</v>
       </c>
       <c r="B45" s="4">
         <f>SIN(A45)</f>
-        <v>0.285520687385303</v>
+        <v>0.7042968673168341</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1741,11 +1748,11 @@
     <row r="46" ht="16" customHeight="1">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
-        <v>1.55044952847966</v>
+        <v>0.8143296573193</v>
       </c>
       <c r="B46" s="4">
         <f>SIN(A46)</f>
-        <v>0.9997930110402919</v>
+        <v>0.727265668271377</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1754,11 +1761,11 @@
     <row r="47" ht="16" customHeight="1">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
-        <v>1.09564838669825</v>
+        <v>0.820047437654828</v>
       </c>
       <c r="B47" s="4">
         <f>SIN(A47)</f>
-        <v>0.889225053197688</v>
+        <v>0.731178191878371</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1767,11 +1774,11 @@
     <row r="48" ht="16" customHeight="1">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
-        <v>-0.741274553729527</v>
+        <v>0.872042507215737</v>
       </c>
       <c r="B48" s="4">
         <f>SIN(A48)</f>
-        <v>-0.67522858154301</v>
+        <v>0.765644404658551</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1780,11 +1787,11 @@
     <row r="49" ht="16" customHeight="1">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
-        <v>-1.10333803654401</v>
+        <v>0.972568216752044</v>
       </c>
       <c r="B49" s="4">
         <f>SIN(A49)</f>
-        <v>-0.892716512550098</v>
+        <v>0.826334803105105</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1793,11 +1800,11 @@
     <row r="50" ht="16" customHeight="1">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
-        <v>1.09743606307681</v>
+        <v>1.00382008465079</v>
       </c>
       <c r="B50" s="4">
         <f>SIN(A50)</f>
-        <v>0.89004144019607</v>
+        <v>0.843528840528085</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -1806,11 +1813,11 @@
     <row r="51" ht="16" customHeight="1">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
-        <v>-0.217792725074985</v>
+        <v>1.01074825445244</v>
       </c>
       <c r="B51" s="4">
         <f>SIN(A51)</f>
-        <v>-0.21607501924673</v>
+        <v>0.847229574669629</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -1819,11 +1826,11 @@
     <row r="52" ht="16" customHeight="1">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
-        <v>-0.0787155310237274</v>
+        <v>1.2454375487267</v>
       </c>
       <c r="B52" s="4">
         <f>SIN(A52)</f>
-        <v>-0.0786342675299594</v>
+        <v>0.947536104436319</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -1832,11 +1839,11 @@
     <row r="53" ht="16" customHeight="1">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
-        <v>-0.462681348450579</v>
+        <v>1.33322544782162</v>
       </c>
       <c r="B53" s="4">
         <f>SIN(A53)</f>
-        <v>-0.446349137152146</v>
+        <v>0.971912516981062</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -1845,11 +1852,11 @@
     <row r="54" ht="16" customHeight="1">
       <c r="A54" s="4">
         <f t="shared" si="0"/>
-        <v>0.249142947491596</v>
+        <v>1.46984391954218</v>
       </c>
       <c r="B54" s="4">
         <f>SIN(A54)</f>
-        <v>0.24657345967081</v>
+        <v>0.994908631948379</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -1858,11 +1865,11 @@
     <row r="55" ht="16" customHeight="1">
       <c r="A55" s="4">
         <f t="shared" si="0"/>
-        <v>-1.36634973841042</v>
+        <v>1.47962346175306</v>
       </c>
       <c r="B55" s="4">
         <f>SIN(A55)</f>
-        <v>-0.979173491018818</v>
+        <v>0.995846632605408</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -1871,11 +1878,11 @@
     <row r="56" ht="16" customHeight="1">
       <c r="A56" s="4">
         <f t="shared" si="0"/>
-        <v>-1.20593243846686</v>
+        <v>1.48085647913658</v>
       </c>
       <c r="B56" s="4">
         <f>SIN(A56)</f>
-        <v>-0.934172337476831</v>
+        <v>0.995958137615362</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -1884,11 +1891,11 @@
     <row r="57" ht="16" customHeight="1">
       <c r="A57" s="4">
         <f t="shared" si="0"/>
-        <v>-0.368777003471654</v>
+        <v>1.4817436937169</v>
       </c>
       <c r="B57" s="4">
         <f>SIN(A57)</f>
-        <v>-0.360474928704474</v>
+        <v>0.996037434027976</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -1897,11 +1904,11 @@
     <row r="58" ht="16" customHeight="1">
       <c r="A58" s="4">
         <f t="shared" si="0"/>
-        <v>-0.0405771229696695</v>
+        <v>1.48497046500358</v>
       </c>
       <c r="B58" s="4">
         <f>SIN(A58)</f>
-        <v>-0.0405659888278309</v>
+        <v>0.9963192209652399</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -1910,11 +1917,11 @@
     <row r="59" ht="16" customHeight="1">
       <c r="A59" s="4">
         <f t="shared" si="0"/>
-        <v>0.452263742204277</v>
+        <v>1.491457713265</v>
       </c>
       <c r="B59" s="4">
         <f>SIN(A59)</f>
-        <v>0.437002797982369</v>
+        <v>0.996854342779614</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -1923,11 +1930,11 @@
     <row r="60" ht="16" customHeight="1">
       <c r="A60" s="4">
         <f t="shared" si="0"/>
-        <v>0.217704619918811</v>
+        <v>1.53142186837804</v>
       </c>
       <c r="B60" s="4">
         <f>SIN(A60)</f>
-        <v>0.215988994580886</v>
+        <v>0.999224926156133</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>

</xml_diff>